<commit_message>
fixed malformed DOI for Eissenberg et al. 1997
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20221123.xlsx
+++ b/inst/suppl_docs/definitions_20221123.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godom\GitHub\CTN-0094\CTNote\inst\suppl_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A923F4-D3A5-4B3D-A882-48FFE065D7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33A3CC1-8980-4432-AA95-6B9B4A2D4975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
@@ -660,9 +660,6 @@
     <t>https://doi.org/10.1001/archpsyc.63.2.210</t>
   </si>
   <si>
-    <t>https://doi.org/10.1001/jama.277.24.1945</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1056/nejmoa055255</t>
   </si>
   <si>
@@ -1005,6 +1002,9 @@
   </si>
   <si>
     <t>Rd_strang_2019</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1001/jama.1997.03540480045037</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1629,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1687,10 +1687,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>8</v>
@@ -1699,7 +1699,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -1713,13 +1713,13 @@
         <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -1728,7 +1728,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
@@ -1757,7 +1757,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
@@ -1774,7 +1774,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -1786,7 +1786,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -1815,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -1832,7 +1832,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
@@ -1844,7 +1844,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
@@ -1873,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
@@ -1890,7 +1890,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>28</v>
@@ -1902,7 +1902,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="204" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>113</v>
@@ -1931,7 +1931,7 @@
         <v>14</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
         <v>83</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -1960,7 +1960,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>32</v>
@@ -1989,7 +1989,7 @@
         <v>14</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2003,10 +2003,10 @@
         <v>109</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>34</v>
@@ -2018,7 +2018,7 @@
         <v>14</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2026,17 +2026,17 @@
         <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>10</v>
@@ -2045,7 +2045,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -2053,17 +2053,17 @@
         <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>10</v>
@@ -2072,7 +2072,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>37</v>
@@ -2101,7 +2101,7 @@
         <v>14</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="130.5" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
@@ -2130,7 +2130,7 @@
         <v>14</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="57" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>42</v>
@@ -2159,7 +2159,7 @@
         <v>14</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>71</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>44</v>
@@ -2188,7 +2188,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2202,10 +2202,10 @@
         <v>109</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>44</v>
@@ -2217,7 +2217,7 @@
         <v>14</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2234,7 +2234,7 @@
         <v>46</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>47</v>
@@ -2246,7 +2246,7 @@
         <v>14</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>51</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>52</v>
@@ -2275,7 +2275,7 @@
         <v>9</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
         <v>53</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>54</v>
@@ -2304,7 +2304,7 @@
         <v>9</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
@@ -2321,7 +2321,7 @@
         <v>56</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>57</v>
@@ -2333,7 +2333,7 @@
         <v>9</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>58</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>114</v>
@@ -2362,7 +2362,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>59</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>60</v>
@@ -2391,7 +2391,7 @@
         <v>119</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="57" x14ac:dyDescent="0.25">
@@ -2407,8 +2407,8 @@
       <c r="D27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>124</v>
+      <c r="E27" t="s">
+        <v>227</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>121</v>
@@ -2420,7 +2420,7 @@
         <v>119</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>63</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>64</v>
@@ -2449,7 +2449,7 @@
         <v>45</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>65</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>66</v>
@@ -2478,7 +2478,7 @@
         <v>45</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
@@ -2492,10 +2492,10 @@
         <v>111</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E30" t="s">
         <v>173</v>
-      </c>
-      <c r="E30" t="s">
-        <v>174</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>69</v>
@@ -2507,7 +2507,7 @@
         <v>9</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J30" s="24"/>
     </row>
@@ -2525,7 +2525,7 @@
         <v>67</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>68</v>
@@ -2537,7 +2537,7 @@
         <v>14</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>69</v>
@@ -2566,7 +2566,7 @@
         <v>25</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>72</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>73</v>
@@ -2595,7 +2595,7 @@
         <v>9</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>75</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>76</v>
@@ -2624,7 +2624,7 @@
         <v>14</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -2638,10 +2638,10 @@
         <v>109</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>78</v>
@@ -2653,7 +2653,7 @@
         <v>9</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>79</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>80</v>
@@ -2682,7 +2682,7 @@
         <v>14</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="57" x14ac:dyDescent="0.25">
@@ -2699,10 +2699,10 @@
         <v>82</v>
       </c>
       <c r="E37" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>40</v>
@@ -2711,7 +2711,7 @@
         <v>9</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="130.5" x14ac:dyDescent="0.25">
@@ -2728,10 +2728,10 @@
         <v>82</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>40</v>
@@ -2740,7 +2740,7 @@
         <v>9</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>83</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>84</v>
@@ -2769,7 +2769,7 @@
         <v>14</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="57" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>85</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>86</v>
@@ -2798,7 +2798,7 @@
         <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
         <v>87</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>88</v>
@@ -2827,7 +2827,7 @@
         <v>14</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="204" x14ac:dyDescent="0.25">
@@ -2844,7 +2844,7 @@
         <v>29</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>89</v>
@@ -2856,7 +2856,7 @@
         <v>14</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
@@ -2873,7 +2873,7 @@
         <v>91</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>92</v>
@@ -2885,7 +2885,7 @@
         <v>14</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>14</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -2931,7 +2931,7 @@
         <v>95</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>96</v>
@@ -2943,7 +2943,7 @@
         <v>120</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2960,7 +2960,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>116</v>
@@ -2972,7 +2972,7 @@
         <v>9</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -2989,7 +2989,7 @@
         <v>7</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>117</v>
@@ -3001,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
@@ -3018,10 +3018,10 @@
         <v>97</v>
       </c>
       <c r="E48" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>10</v>
@@ -3030,7 +3030,7 @@
         <v>9</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.25">
@@ -3047,10 +3047,10 @@
         <v>97</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>10</v>
@@ -3059,7 +3059,7 @@
         <v>14</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="57" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>98</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>99</v>
@@ -3088,7 +3088,7 @@
         <v>14</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>23</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>100</v>
@@ -3117,7 +3117,7 @@
         <v>25</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>101</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>84</v>
@@ -3146,7 +3146,7 @@
         <v>25</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="57" x14ac:dyDescent="0.25">
@@ -3163,7 +3163,7 @@
         <v>102</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>103</v>
@@ -3175,10 +3175,10 @@
         <v>119</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>104</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>105</v>
@@ -3204,7 +3204,7 @@
         <v>14</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the reduction entry of the library and the table so that reduction outcomes are (mostly) corrected to have the prefix "Rd" instead of "Ab". There is one definition that should still be labelled as "Ab" despite being included in the reduction section.
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20221123.xlsx
+++ b/inst/suppl_docs/definitions_20221123.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godom\GitHub\CTN-0094\CTNote\inst\suppl_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33A3CC1-8980-4432-AA95-6B9B4A2D4975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1A6505-3459-104D-B124-AE918AD2D9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
+    <workbookView xWindow="340" yWindow="520" windowWidth="32420" windowHeight="19240" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,9 +630,6 @@
     <t>No evidence of opioid use based on UOS (NOTE: minimal evidence of opioid use from UOS, not none)</t>
   </si>
   <si>
-    <t>Index of illicit morphine use ([0, 120])</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -899,41 +896,7 @@
     <t>Rd_johnson_1992</t>
   </si>
   <si>
-    <t>Ab_soyka_2008</t>
-  </si>
-  <si>
     <t>Ab_schwartz_2006</t>
-  </si>
-  <si>
-    <t>Ab_strain_1996</t>
-  </si>
-  <si>
-    <t>Ab_lingA_1976</t>
-  </si>
-  <si>
-    <t>Ab_woody_2008</t>
-  </si>
-  <si>
-    <t>Ab_eissenberg_1997</t>
-  </si>
-  <si>
-    <t>Ab_strain_1993</t>
-  </si>
-  <si>
-    <t>Ab_zaks_1972</t>
-  </si>
-  <si>
-    <t>Ab_strain_1999</t>
-  </si>
-  <si>
-    <t>Ab_petitjean_2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-Ab_shufman_1994</t>
-  </si>
-  <si>
-    <t>Ab_strain_1994</t>
   </si>
   <si>
     <t>Rd_strang_2010</t>
@@ -1005,6 +968,43 @@
   </si>
   <si>
     <t>https://doi.org/10.1001/jama.1997.03540480045037</t>
+  </si>
+  <si>
+    <t>Index of illicit morphine use ([0, 120]). Note: this is a complex definition; for details see the original paper.</t>
+  </si>
+  <si>
+    <t>Rd_eissenberg_1997</t>
+  </si>
+  <si>
+    <t>Rd_lingA_1976</t>
+  </si>
+  <si>
+    <t>Rd_petitjean_2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+Rd_shufman_1994</t>
+  </si>
+  <si>
+    <t>Rd_soyka_2008</t>
+  </si>
+  <si>
+    <t>Rd_strain_1993</t>
+  </si>
+  <si>
+    <t>Rd_strain_1994</t>
+  </si>
+  <si>
+    <t>Rd_strain_1996</t>
+  </si>
+  <si>
+    <t>Rd_strain_1999</t>
+  </si>
+  <si>
+    <t>Rd_woody_2008</t>
+  </si>
+  <si>
+    <t>Rd_zaks_1972</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1618,7 +1618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1628,23 +1628,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="49.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
     <col min="9" max="9" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>107</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>2</v>
@@ -1673,7 +1673,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -1687,10 +1687,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>8</v>
@@ -1699,10 +1699,10 @@
         <v>9</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1713,13 +1713,13 @@
         <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -1728,10 +1728,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
@@ -1757,10 +1757,10 @@
         <v>14</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="47" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -1786,10 +1786,10 @@
         <v>25</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -1815,10 +1815,10 @@
         <v>14</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
@@ -1844,10 +1844,10 @@
         <v>14</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
@@ -1873,10 +1873,10 @@
         <v>25</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>28</v>
@@ -1902,10 +1902,10 @@
         <v>14</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>113</v>
@@ -1931,10 +1931,10 @@
         <v>14</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>83</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -1960,10 +1960,10 @@
         <v>14</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
@@ -1977,22 +1977,22 @@
         <v>27</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2003,10 @@
         <v>109</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>34</v>
@@ -2018,25 +2018,25 @@
         <v>14</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>10</v>
@@ -2045,25 +2045,25 @@
         <v>14</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>10</v>
@@ -2072,10 +2072,10 @@
         <v>25</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>35</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>37</v>
@@ -2101,10 +2101,10 @@
         <v>14</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="130.5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>35</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
@@ -2130,10 +2130,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>35</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>42</v>
@@ -2159,10 +2159,10 @@
         <v>14</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>35</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>71</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>44</v>
@@ -2188,10 +2188,10 @@
         <v>14</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>35</v>
       </c>
@@ -2202,10 +2202,10 @@
         <v>109</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>44</v>
@@ -2217,10 +2217,10 @@
         <v>14</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>35</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>46</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>47</v>
@@ -2246,10 +2246,10 @@
         <v>14</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>49</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>51</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>52</v>
@@ -2275,10 +2275,10 @@
         <v>9</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>49</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>53</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>54</v>
@@ -2304,10 +2304,10 @@
         <v>9</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>49</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>56</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>57</v>
@@ -2333,10 +2333,10 @@
         <v>9</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>49</v>
       </c>
@@ -2350,10 +2350,10 @@
         <v>58</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>10</v>
@@ -2362,10 +2362,10 @@
         <v>14</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>59</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>60</v>
@@ -2388,13 +2388,13 @@
         <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>49</v>
       </c>
@@ -2408,22 +2408,22 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>49</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>63</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>64</v>
@@ -2449,10 +2449,10 @@
         <v>45</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>49</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>65</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>66</v>
@@ -2478,10 +2478,10 @@
         <v>45</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>49</v>
       </c>
@@ -2492,10 +2492,10 @@
         <v>111</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" t="s">
         <v>172</v>
-      </c>
-      <c r="E30" t="s">
-        <v>173</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>69</v>
@@ -2507,11 +2507,11 @@
         <v>9</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="J30" s="24"/>
     </row>
-    <row r="31" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>49</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>67</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>68</v>
@@ -2537,10 +2537,10 @@
         <v>14</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>49</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>69</v>
@@ -2566,10 +2566,10 @@
         <v>25</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>49</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>72</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>73</v>
@@ -2595,10 +2595,10 @@
         <v>9</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>49</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>75</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>76</v>
@@ -2624,10 +2624,10 @@
         <v>14</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>49</v>
       </c>
@@ -2638,10 +2638,10 @@
         <v>109</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>78</v>
@@ -2653,10 +2653,10 @@
         <v>9</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>49</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>79</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>80</v>
@@ -2682,10 +2682,10 @@
         <v>14</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>49</v>
       </c>
@@ -2699,10 +2699,10 @@
         <v>82</v>
       </c>
       <c r="E37" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>40</v>
@@ -2711,10 +2711,10 @@
         <v>9</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="130.5" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
@@ -2728,10 +2728,10 @@
         <v>82</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>40</v>
@@ -2740,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>49</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>83</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>84</v>
@@ -2769,10 +2769,10 @@
         <v>14</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>49</v>
       </c>
@@ -2780,13 +2780,13 @@
         <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>86</v>
@@ -2798,10 +2798,10 @@
         <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>49</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>87</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>88</v>
@@ -2827,10 +2827,10 @@
         <v>14</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>49</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>29</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>89</v>
@@ -2856,10 +2856,10 @@
         <v>14</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>49</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>91</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>92</v>
@@ -2885,10 +2885,10 @@
         <v>14</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>93</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>94</v>
@@ -2914,10 +2914,10 @@
         <v>14</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>49</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>95</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>96</v>
@@ -2940,13 +2940,13 @@
         <v>10</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>49</v>
       </c>
@@ -2960,10 +2960,10 @@
         <v>7</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>8</v>
@@ -2972,10 +2972,10 @@
         <v>9</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>49</v>
       </c>
@@ -2989,10 +2989,10 @@
         <v>7</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>8</v>
@@ -3001,10 +3001,10 @@
         <v>9</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>49</v>
       </c>
@@ -3018,10 +3018,10 @@
         <v>97</v>
       </c>
       <c r="E48" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>10</v>
@@ -3030,10 +3030,10 @@
         <v>9</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>49</v>
       </c>
@@ -3047,10 +3047,10 @@
         <v>97</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>10</v>
@@ -3059,10 +3059,10 @@
         <v>14</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>49</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>98</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>99</v>
@@ -3088,10 +3088,10 @@
         <v>14</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>49</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>23</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>100</v>
@@ -3117,10 +3117,10 @@
         <v>25</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>49</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>101</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>84</v>
@@ -3146,10 +3146,10 @@
         <v>25</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>49</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>102</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>103</v>
@@ -3172,13 +3172,13 @@
         <v>8</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>104</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>105</v>
@@ -3204,7 +3204,7 @@
         <v>14</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>